<commit_message>
EPBDS-4097 Deployment isolation feature, fix bug in class loader isolation
</commit_message>
<xml_diff>
--- a/WSFrontend/trunk/org.openl.rules.ruleservice/test-resources/domain-sharing-multimodule/project2/Module2_1.xlsx
+++ b/WSFrontend/trunk/org.openl.rules.ruleservice/test-resources/domain-sharing-multimodule/project2/Module2_1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="19035" windowHeight="10995"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Environment</t>
   </si>
@@ -31,53 +31,56 @@
     <t>domain</t>
   </si>
   <si>
+    <t>Method String print(TestDatatype datatype)</t>
+  </si>
+  <si>
+    <t>Method String printJavaBean()</t>
+  </si>
+  <si>
+    <t>return "project2"+print(datatypes[0]);</t>
+  </si>
+  <si>
+    <t>Method String printDatatype()</t>
+  </si>
+  <si>
+    <t>stringField</t>
+  </si>
+  <si>
+    <t>javabean</t>
+  </si>
+  <si>
+    <t>doubleField</t>
+  </si>
+  <si>
+    <t>return bean.stringField + bean.doubleField;</t>
+  </si>
+  <si>
+    <t>return datatype.stringValue + datatype.boolValue;</t>
+  </si>
+  <si>
+    <t>import</t>
+  </si>
+  <si>
+    <t>org.openl.example2</t>
+  </si>
+  <si>
+    <t>Method String printJavaBeanSecond()</t>
+  </si>
+  <si>
+    <t>return "project2"+print(beans2[0]);</t>
+  </si>
+  <si>
     <t>Method String print(TestBean bean)</t>
   </si>
   <si>
-    <t>Method String print(TestDatatype datatype)</t>
-  </si>
-  <si>
-    <t>Method String printJavaBean()</t>
-  </si>
-  <si>
-    <t>return "project2"+print(beans[0]);</t>
-  </si>
-  <si>
-    <t>return "project2"+print(datatypes[0]);</t>
-  </si>
-  <si>
-    <t>Method String printDatatype()</t>
-  </si>
-  <si>
-    <t>Data TestBean beans</t>
-  </si>
-  <si>
-    <t>stringField</t>
-  </si>
-  <si>
-    <t>javabean</t>
-  </si>
-  <si>
-    <t>doubleField</t>
-  </si>
-  <si>
-    <t>return bean.stringField + bean.doubleField;</t>
-  </si>
-  <si>
-    <t>return datatype.stringValue + datatype.boolValue;</t>
-  </si>
-  <si>
-    <t>import</t>
-  </si>
-  <si>
-    <t>org.openl.example</t>
+    <t>Data TestBean beans2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -220,11 +223,16 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Vehicle-Eligibility"/>
@@ -352,6 +360,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -386,6 +395,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -561,14 +571,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:G21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="F4" sqref="F4:G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.85546875" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="28.140625" customWidth="1" collapsed="1"/>
@@ -578,122 +588,138 @@
     <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
     </row>
-    <row r="4" spans="2:7">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
       <c r="F4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="9"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="9"/>
-    </row>
-    <row r="5" spans="2:7">
-      <c r="F5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7">
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F6" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G6" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:7">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
       <c r="F7" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G7" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:7">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="10" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
     </row>
-    <row r="11" spans="2:7">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
     </row>
-    <row r="12" spans="2:7">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
     </row>
-    <row r="15" spans="2:7">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
     </row>
-    <row r="16" spans="2:7">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
     </row>
-    <row r="19" spans="2:3">
-      <c r="B19" s="8" t="s">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C19" s="9"/>
-    </row>
-    <row r="20" spans="2:3">
-      <c r="B20" s="2" t="s">
+      <c r="C21" s="9"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="2:3">
-      <c r="B21" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>16</v>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="12">
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B21:C21"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>